<commit_message>
test case in progress
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEVELOPER\Documents\UiPath\DataCleaner\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEVELOPER\Documents\UiPath\RPA_BAG_SOSR_DataCleaner\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD67AF4C-EEE6-4459-8474-9DAEAFBDFEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAE3E48-CD58-4124-AA64-340FDA9189ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2838,8 +2838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Before chandes in Hotels Rooms Option
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEVELOPER\Documents\UiPath\RPA_BAG_SOSR_DataCleaner\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAE3E48-CD58-4124-AA64-340FDA9189ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BAC1D0-E1D7-4BDF-8F96-24AAF94B2718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1668,7 +1668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -2838,7 +2838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>